<commit_message>
#39 Prepared Excel Testdata
</commit_message>
<xml_diff>
--- a/cintamani-next/data/products/products.xlsx
+++ b/cintamani-next/data/products/products.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -53,16 +53,37 @@
     <t>Aksobhya Kupferstatue 21cm</t>
   </si>
   <si>
-    <t>sehr fein gearbeitete Kupferstatue</t>
-  </si>
-  <si>
     <t>cintamani275_7</t>
   </si>
   <si>
-    <t>Aksobhya Anders 21cm</t>
-  </si>
-  <si>
-    <t>andere Figur</t>
+    <t>Buddhas - Manjusri</t>
+  </si>
+  <si>
+    <t>manjusri</t>
+  </si>
+  <si>
+    <t>Malas  - klein</t>
+  </si>
+  <si>
+    <t>Thangkas  - groß</t>
+  </si>
+  <si>
+    <t>kleine mala</t>
+  </si>
+  <si>
+    <t>große Thangka</t>
+  </si>
+  <si>
+    <t>große Thangka 2</t>
+  </si>
+  <si>
+    <t>Thangkas  - klein</t>
+  </si>
+  <si>
+    <t>kleine thangka</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
   </si>
 </sst>
 </file>
@@ -414,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,10 +491,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -481,22 +502,114 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3">
+        <v>649</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
         <v>250</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>12</v>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>250</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>250</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>